<commit_message>
fs alert for excel update
</commit_message>
<xml_diff>
--- a/specs/excel/GameConfig.xlsx
+++ b/specs/excel/GameConfig.xlsx
@@ -28,7 +28,7 @@
     <t>字段值</t>
   </si>
   <si>
-    <t>描述</t>
+    <t>描述#desc</t>
   </si>
   <si>
     <t>Id</t>
@@ -1133,7 +1133,7 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>

</xml_diff>